<commit_message>
convert all values in input values INPUTS_CALCULATION_MODULE to strings
</commit_message>
<xml_diff>
--- a/cm/app/api_v1/my_calculation_module_directory/INPUTS_CALCULATION_MODULE.xlsx
+++ b/cm/app/api_v1/my_calculation_module_directory/INPUTS_CALCULATION_MODULE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasani\Documents\Workplace\Hotmaps\dispatch_module\cm\app\api_v1\my_calculation_module_directory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9058D5-2349-448D-A04D-CC71562A27E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1DE1C9-621E-4D56-AD05-39394C1FE9C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{A39C18F9-790E-4AC0-B0AE-6D70F2BE89C8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="131">
   <si>
     <t>input_name</t>
   </si>
@@ -394,9 +394,6 @@
   </si>
   <si>
     <t>pCO2_pCO2</t>
-  </si>
-  <si>
-    <t>radio </t>
   </si>
   <si>
     <t>["invest","dispatch"]</t>
@@ -791,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED82753-5272-4518-B7D2-E7729D132D1F}">
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +862,7 @@
         <v>100000</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -894,7 +891,7 @@
         <v>100000</v>
       </c>
       <c r="I3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -923,7 +920,7 @@
         <v>100000</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -952,7 +949,7 @@
         <v>100000</v>
       </c>
       <c r="I5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -981,7 +978,7 @@
         <v>100000</v>
       </c>
       <c r="I6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1010,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1039,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1068,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1097,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1126,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1155,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1184,7 +1181,7 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1213,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1242,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1271,7 +1268,7 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1285,7 +1282,7 @@
         <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1300,7 +1297,7 @@
         <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1314,7 +1311,7 @@
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1329,7 +1326,7 @@
         <v>12</v>
       </c>
       <c r="I18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1343,7 +1340,7 @@
         <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1358,7 +1355,7 @@
         <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1372,7 +1369,7 @@
         <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E20">
         <v>3</v>
@@ -1387,7 +1384,7 @@
         <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1401,7 +1398,7 @@
         <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1416,7 +1413,7 @@
         <v>12</v>
       </c>
       <c r="I21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1445,7 +1442,7 @@
         <v>10000000</v>
       </c>
       <c r="I22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1474,7 +1471,7 @@
         <v>10000000</v>
       </c>
       <c r="I23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1503,7 +1500,7 @@
         <v>10000000</v>
       </c>
       <c r="I24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1532,7 +1529,7 @@
         <v>10000000</v>
       </c>
       <c r="I25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1561,7 +1558,7 @@
         <v>10000000</v>
       </c>
       <c r="I26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1590,7 +1587,7 @@
         <v>10000000</v>
       </c>
       <c r="I27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1619,7 +1616,7 @@
         <v>10000000</v>
       </c>
       <c r="I28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1648,7 +1645,7 @@
         <v>10000000</v>
       </c>
       <c r="I29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1677,7 +1674,7 @@
         <v>10000000</v>
       </c>
       <c r="I30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1706,7 +1703,7 @@
         <v>10000000</v>
       </c>
       <c r="I31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1735,7 +1732,7 @@
         <v>10000000</v>
       </c>
       <c r="I32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1764,7 +1761,7 @@
         <v>10000000</v>
       </c>
       <c r="I33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1793,7 +1790,7 @@
         <v>10000000</v>
       </c>
       <c r="I34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1822,7 +1819,7 @@
         <v>10000000</v>
       </c>
       <c r="I35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1851,7 +1848,7 @@
         <v>10000000</v>
       </c>
       <c r="I36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1880,7 +1877,7 @@
         <v>50</v>
       </c>
       <c r="I37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1909,7 +1906,7 @@
         <v>50</v>
       </c>
       <c r="I38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1938,7 +1935,7 @@
         <v>50</v>
       </c>
       <c r="I39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1967,7 +1964,7 @@
         <v>50</v>
       </c>
       <c r="I40" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1996,7 +1993,7 @@
         <v>50</v>
       </c>
       <c r="I41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2025,18 +2022,18 @@
         <v>100000</v>
       </c>
       <c r="I42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
         <v>127</v>
-      </c>
-      <c r="B43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" t="s">
-        <v>128</v>
       </c>
       <c r="D43">
         <v>100</v>
@@ -2054,7 +2051,7 @@
         <v>100000</v>
       </c>
       <c r="I43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2083,7 +2080,7 @@
         <v>100000</v>
       </c>
       <c r="I44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2094,7 +2091,7 @@
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D45">
         <v>36</v>
@@ -2112,7 +2109,7 @@
         <v>100000</v>
       </c>
       <c r="I45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2141,7 +2138,7 @@
         <v>100000</v>
       </c>
       <c r="I46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2170,7 +2167,7 @@
         <v>100000</v>
       </c>
       <c r="I47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2199,7 +2196,7 @@
         <v>100000</v>
       </c>
       <c r="I48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2210,7 +2207,7 @@
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -2228,7 +2225,7 @@
         <v>100000</v>
       </c>
       <c r="I49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -2257,7 +2254,7 @@
         <v>100000</v>
       </c>
       <c r="I50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -2268,7 +2265,7 @@
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -2286,7 +2283,7 @@
         <v>100000</v>
       </c>
       <c r="I51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -2315,7 +2312,7 @@
         <v>100000</v>
       </c>
       <c r="I52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -2344,7 +2341,7 @@
         <v>100000</v>
       </c>
       <c r="I53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2373,7 +2370,7 @@
         <v>100000</v>
       </c>
       <c r="I54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -2402,7 +2399,7 @@
         <v>12</v>
       </c>
       <c r="I55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
@@ -2410,13 +2407,13 @@
         <v>85</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="C56" t="s">
         <v>121</v>
       </c>
       <c r="D56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -2431,7 +2428,7 @@
         <v>12</v>
       </c>
       <c r="I56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>